<commit_message>
change cholesterol discr e0e672ed2872335af873328990ab31d37329a62f
</commit_message>
<xml_diff>
--- a/nr-add-lipids/ig/StructureDefinition-mesures-bundle-flux-alimentation-cholesterol.xlsx
+++ b/nr-add-lipids/ig/StructureDefinition-mesures-bundle-flux-alimentation-cholesterol.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-13T13:38:24+00:00</t>
+    <t>2024-12-13T13:39:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -605,7 +605,7 @@
     <t>An entry in a bundle resource - will either contain a resource or information about a resource (transactions and history only).</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:request.url}
+    <t xml:space="preserve">profile:resource}
 </t>
   </si>
   <si>

</xml_diff>